<commit_message>
rotate xtrics and consider cases diagnosed directly by dockers
</commit_message>
<xml_diff>
--- a/huanggang/20200212.xlsx
+++ b/huanggang/20200212.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="13720" yWindow="1100" windowWidth="25600" windowHeight="14240"/>
+    <workbookView xWindow="9780" yWindow="2500" windowWidth="25600" windowHeight="14180"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -125,7 +125,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="3" x14ac:knownFonts="1">
+  <fonts count="5" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color rgb="FF000000"/>
@@ -139,6 +139,20 @@
     </font>
     <font>
       <sz val="9"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color theme="10"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color theme="11"/>
       <name val="Calibri"/>
       <family val="2"/>
     </font>
@@ -167,8 +181,10 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
   <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
@@ -183,7 +199,9 @@
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="3">
+    <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="1" builtinId="8" hidden="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -499,7 +517,7 @@
   <dimension ref="A1:E14"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D19" sqref="D19"/>
+      <selection activeCell="C8" sqref="C8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -745,5 +763,6 @@
   </mergeCells>
   <phoneticPr fontId="2" type="noConversion"/>
   <pageMargins left="1.25" right="1.25" top="1" bottom="0.79166666666666696" header="0.25" footer="0.25"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="0" verticalDpi="0"/>
 </worksheet>
 </file>
</xml_diff>